<commit_message>
Added in vernacular citations as per #15 . Also, refactored pagination into web- and print- specific functions, as a way of dealing with pagination aspects that are currently baked into code (eg policy checklist completion), for #14
</commit_message>
<xml_diff>
--- a/_report_configuration.xlsx
+++ b/_report_configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2659" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D9166CC-EFCF-4CC8-A41B-9FF6981A1C58}"/>
+  <xr:revisionPtr revIDLastSave="2706" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519D5011-1A61-4968-ABF5-CDDB4C5C9F0E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5278" uniqueCount="2031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5278" uniqueCount="2043">
   <si>
     <t>name</t>
   </si>
@@ -6245,10 +6245,46 @@
 ยั่งยืนสำหรับ 25 เมืองใน 19 ประเทศ</t>
   </si>
   <si>
-    <t>{"study_citations":"||The Lancet Global Health. May 2022. Volume 10. Special Issue 2. Urban Design, Transport and Health Series II. S1-S5.","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({language}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
-  </si>
-  <si>
     <t>2018 Scholar44 (Wikimedia Commons) under CC0 1.0 Universal licence</t>
+  </si>
+  <si>
+    <t>{"study_citations":"||The Lancet Global Health. May 2022. Volume 10. Special Issue 2. Urban Design, Transport and Health Series II. S1-S5.","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({vernacular}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
+  </si>
+  <si>
+    <t>{"German":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Vietnamese":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Thai":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Tamil":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Dutch":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Czech":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Danish":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Catalan":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}","Spanish - Spain":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Portuguese - Brazil":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Portuguese - Portugal":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Spanish - Mexico":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
+  </si>
+  <si>
+    <t>{"Hausa":"{'citation_doi':'Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {title_series_line1}:{title_series_line2} ({city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally, {language}; translated by {translation_names}). {city_doi}'}"}</t>
   </si>
 </sst>
 </file>
@@ -7198,16 +7234,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
@@ -7371,6 +7397,16 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7700,7 +7736,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G182" sqref="G182"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P2:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7814,10 +7850,6 @@
       <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A2,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q2">
         <v>5</v>
       </c>
@@ -7878,10 +7910,6 @@
       <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="P3" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A3,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q3">
         <v>5</v>
       </c>
@@ -7942,10 +7970,6 @@
       <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A4,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q4">
         <v>5</v>
       </c>
@@ -8005,10 +8029,6 @@
       </c>
       <c r="O5" t="s">
         <v>22</v>
-      </c>
-      <c r="P5" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A5,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
       </c>
       <c r="Q5">
         <v>5</v>
@@ -19278,10 +19298,10 @@
   <dimension ref="A1:V195"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19395,10 +19415,6 @@
       <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_print!A2,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q2">
         <v>5</v>
       </c>
@@ -19459,10 +19475,6 @@
       <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="P3" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_print!A3,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q3">
         <v>5</v>
       </c>
@@ -19523,10 +19535,6 @@
       <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_print!A4,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
-      </c>
       <c r="Q4">
         <v>5</v>
       </c>
@@ -19586,10 +19594,6 @@
       </c>
       <c r="O5" t="s">
         <v>22</v>
-      </c>
-      <c r="P5" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_print!A5,languages!B:B,0)),"")</f>
-        <v>{city}, {country}</v>
       </c>
       <c r="Q5">
         <v>5</v>
@@ -30844,7 +30848,7 @@
   </sheetData>
   <autoFilter ref="A1:T192" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30859,10 +30863,10 @@
   <dimension ref="A1:V171"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S88" sqref="S88"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39325,25 +39329,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B107:D109 L98:L99 N98:V99 G107:J109 L92:V97 B1:V86 K124:K171 B92:J106 L100:V120 L123:V171 B110:J120 B123:J171 K92:K120 B121:V123 B88:V91">
-    <cfRule type="containsBlanks" dxfId="23" priority="46">
+    <cfRule type="containsBlanks" dxfId="22" priority="46">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M98:M99">
-    <cfRule type="containsBlanks" dxfId="22" priority="4">
+    <cfRule type="containsBlanks" dxfId="21" priority="4">
       <formula>LEN(TRIM(M98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B86 B88:B171">
-    <cfRule type="duplicateValues" dxfId="21" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87:V87">
-    <cfRule type="containsBlanks" dxfId="20" priority="1">
+    <cfRule type="containsBlanks" dxfId="19" priority="1">
       <formula>LEN(TRIM(B87))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -39358,10 +39362,10 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39429,10 +39433,10 @@
         <v>1932</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>2029</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>186</v>
       </c>
@@ -39457,11 +39461,11 @@
       <c r="H3" s="48" t="s">
         <v>1945</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>181</v>
       </c>
@@ -39486,8 +39490,8 @@
       <c r="H4" s="48" t="s">
         <v>1933</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>1629</v>
+      <c r="I4" s="3" t="s">
+        <v>2041</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -39602,8 +39606,8 @@
       <c r="H8" s="48" t="s">
         <v>1941</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>1629</v>
+      <c r="I8" s="3" t="s">
+        <v>2039</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -39635,7 +39639,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>192</v>
       </c>
@@ -39660,11 +39664,11 @@
       <c r="H10" s="48" t="s">
         <v>1952</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>180</v>
       </c>
@@ -39689,11 +39693,11 @@
       <c r="H11" s="48" t="s">
         <v>1956</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>193</v>
       </c>
@@ -39718,8 +39722,8 @@
       <c r="H12" s="48" t="s">
         <v>1948</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>1629</v>
+      <c r="I12" s="3" t="s">
+        <v>2032</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -39747,11 +39751,11 @@
       <c r="H13" s="48" t="s">
         <v>1949</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>195</v>
       </c>
@@ -39776,8 +39780,8 @@
       <c r="H14" s="48" t="s">
         <v>1950</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>1629</v>
+      <c r="I14" s="3" t="s">
+        <v>2035</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -39805,11 +39809,11 @@
       <c r="H15" s="48" t="s">
         <v>1953</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>197</v>
       </c>
@@ -39834,8 +39838,8 @@
       <c r="H16" s="48" t="s">
         <v>1943</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>1629</v>
+      <c r="I16" s="3" t="s">
+        <v>2036</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -39863,11 +39867,11 @@
       <c r="H17" s="48" t="s">
         <v>1951</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>199</v>
       </c>
@@ -39892,11 +39896,11 @@
       <c r="H18" s="48" t="s">
         <v>1934</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>200</v>
       </c>
@@ -39921,11 +39925,11 @@
       <c r="H19" s="48" t="s">
         <v>1955</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I19" s="3" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>201</v>
       </c>
@@ -39950,11 +39954,11 @@
       <c r="H20" s="48" t="s">
         <v>1938</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I20" s="3" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>202</v>
       </c>
@@ -39979,8 +39983,8 @@
       <c r="H21" s="48" t="s">
         <v>1937</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>1629</v>
+      <c r="I21" s="3" t="s">
+        <v>2038</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -40012,7 +40016,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>204</v>
       </c>
@@ -40037,8 +40041,8 @@
       <c r="H23" s="48" t="s">
         <v>1946</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>1629</v>
+      <c r="I23" s="3" t="s">
+        <v>2040</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="300" x14ac:dyDescent="0.25">
@@ -40055,7 +40059,7 @@
         <v>2010</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>1982</v>
@@ -40602,8 +40606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0E5A34-E8C6-471F-BB3C-81719394AD1E}">
   <dimension ref="A2:U29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41360,11 +41364,11 @@
       <c r="A14" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="52" t="str">
+      <c r="B14" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>Graz, Austria-14.09.2020: people relaxing outdoor in a park near Mur river, in summer, Styria region, Austria. Selective focus.</v>
       </c>
-      <c r="C14" s="52" t="str">
+      <c r="C14" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>Graz, Austria - June 16, 2020 - cyclists and pedestrians in front of modern tram street car next to traditional Austrian houses</v>
       </c>
@@ -41488,11 +41492,11 @@
       <c r="A16" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="52" t="str">
+      <c r="B16" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>BERN, SWITZERLAND - APRIL 15, 2018: Street view on Kramgasse with fountain and clock tower in the old town of Bern city.It is a popular shopping street and medieval city centre of Bern, Switzerland</v>
       </c>
-      <c r="C16" s="52" t="str">
+      <c r="C16" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>Bern Switzerland , 27 June 2020 : Pedestrian street with cafe terrace full of people during summer 2020 in Bern old town Switzerland</v>
       </c>
@@ -41620,11 +41624,11 @@
       <c r="A18" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="52" t="str">
+      <c r="B18" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>COLOGNE,NORTH RHINE WESTPHALIA,GERMANY - FEBRUARY 14 2021: People ice skating in German park at winter</v>
       </c>
-      <c r="C18" s="52" t="str">
+      <c r="C18" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>Cologne, Germany - 15 June 2019: The Great Saint Martin Church and Colorful buildings nearby riverside of Hohenzollern Bridge in Cologne.</v>
       </c>
@@ -42075,8 +42079,14 @@
       <c r="A25" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="35" t="str">
+        <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A25,city_details!A:A,0))</f>
+        <v>This photo of an Adelaide tram was taken at the southern end of King William Street, Adelaide, South Australia, looking south across South Terrace. An Adelaide Metro tram (Alstom Citadis 302 model, number 206) is at the northern end of the 9.3 kilometre sole-use reservation of the Adelaide–Glenelg tram line. From here it will leave the reservation and, crossing South Terrace, run on the street tramlines of central Adelaide.</v>
+      </c>
+      <c r="C25" s="35" t="str">
+        <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A25,city_details!A:A,0))</f>
+        <v>Adelaide City Skyline during 2022 Australia Day Celebrations</v>
+      </c>
       <c r="D25" s="41" t="s">
         <v>818</v>
       </c>
@@ -42337,68 +42347,68 @@
     <mergeCell ref="E2:T2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C28">
-    <cfRule type="containsBlanks" dxfId="18" priority="18">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P28">
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",P4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="Auto">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Auto">
       <formula>NOT(ISERROR(SEARCH("Auto",P4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",P4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D28">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="Auto">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Auto">
       <formula>NOT(ISERROR(SEARCH("Auto",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:T28">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"???"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Partial"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="Auto">
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="Auto">
       <formula>NOT(ISERROR(SEARCH("Auto",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Auto">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Auto">
       <formula>NOT(ISERROR(SEARCH("Auto",N9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",N9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",T13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Auto">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Auto">
       <formula>NOT(ISERROR(SEARCH("Auto",T13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",T13)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated The Lancet Global Health series citation
</commit_message>
<xml_diff>
--- a/_report_configuration.xlsx
+++ b/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3122" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2099B4A6-57FC-4F3E-9A87-2E4B512FEB1A}"/>
+  <xr:revisionPtr revIDLastSave="3128" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F644FC8-1775-4DED-8EDE-B797BB5A9D4A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_web" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5277" uniqueCount="2052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5277" uniqueCount="2051">
   <si>
     <t>name</t>
   </si>
@@ -5623,9 +5623,6 @@
   </si>
   <si>
     <t>To be updated on sunny day</t>
-  </si>
-  <si>
-    <t>partial</t>
   </si>
   <si>
     <t>{"English":"{'local_collaborators_names':'Claire Cleland, Sara Ferguson &amp; Ruth Hunter||For further information, please contact ruth.hunter@qub.ac.uk'}"}</t>
@@ -6184,9 +6181,6 @@
     <t>2018 Scholar44 (Wikimedia Commons) under CC0 1.0 Universal licence</t>
   </si>
   <si>
-    <t>{"study_citations":"||The Lancet Global Health. May 2022. Volume 10. Special Issue 2. Urban Design, Transport and Health Series II. S1-S5.","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({vernacular}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
-  </si>
-  <si>
     <t>The availability of urban and transport policies supporting health and sustainability in Adelaide is above average compared with other cities studied. However, the quality of those policies is below average. Adelaide does not appear to have transport planning policies incorporating health-focussed actions or air pollution policies related to transport or land use planning. Nor does it require health impact assessement of transport and land use interventions. Adelaide's targets for walking and cycling participation and public transport use are too low to be consistent with healthy cities evidence. Hence, relative to the 25 cities in this international study, the vast majority of neighbourhoods in Adelaide have low walkability. In terms of thresholds to achieve WHO targets to increase physical activity, no neighbourhoods in Adelaide achieve population density thresholds and only 13% achieve street connectivity thresholds. Only 54% of residents have nearby access to public transport stops with regular services. The majority of residents have some public open space within 500m. However, this drops to only 58% who have access to larger public open space, and access is spatially patterned. Compared with the other cities studied, the proportion of the population in Adelaide with access within 500m to a food market, convenience store and, to a lesser extent, public transport stop with a regular service is below average.</t>
   </si>
   <si>
@@ -6313,6 +6307,9 @@
   </si>
   <si>
     <t>Vergleiche mit den Medianwerten aller Städte dieser internationalen Studie könnten zu den für die lokale Stadtpolitik erforderlichen Änderungen führen. Die Karten zeigen die Verteilung von Stadtgestaltung und Verkehrsmerkmalen in {city} und identifizieren Gebiete, die am meisten von Interventionen profitieren könnten, um eine gesunde und nachhaltige Umwelt zu schaffen.</t>
+  </si>
+  <si>
+    <t>{"study_citations":"||The Lancet Global Health Series on urban design, transport, and health. 2022. https://www.thelancet.com/series/urban-design-2022 ","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({vernacular}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
   </si>
 </sst>
 </file>
@@ -8456,7 +8453,7 @@
         <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="Q12">
         <v>3</v>
@@ -8514,7 +8511,7 @@
         <v>28</v>
       </c>
       <c r="P13" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -9211,7 +9208,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -9834,10 +9831,10 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="N36" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O36" t="s">
         <v>26</v>
@@ -9896,7 +9893,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O37" t="s">
         <v>26</v>
@@ -9956,7 +9953,7 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -10013,7 +10010,7 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O39" t="s">
         <v>26</v>
@@ -10073,7 +10070,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O40" t="s">
         <v>28</v>
@@ -10134,7 +10131,7 @@
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>28</v>
@@ -10196,7 +10193,7 @@
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>28</v>
@@ -10254,7 +10251,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O43" t="s">
         <v>26</v>
@@ -10310,7 +10307,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O44" t="s">
         <v>26</v>
@@ -10370,7 +10367,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O45" t="s">
         <v>26</v>
@@ -10433,7 +10430,7 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O46" t="s">
         <v>26</v>
@@ -10493,7 +10490,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O47" t="s">
         <v>28</v>
@@ -10557,7 +10554,7 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O48" t="s">
         <v>28</v>
@@ -10619,7 +10616,7 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O49" t="s">
         <v>28</v>
@@ -10680,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O50" t="s">
         <v>26</v>
@@ -10743,7 +10740,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O51" t="s">
         <v>26</v>
@@ -10803,7 +10800,7 @@
         <v>0</v>
       </c>
       <c r="N52" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O52" t="s">
         <v>28</v>
@@ -10867,7 +10864,7 @@
         <v>0</v>
       </c>
       <c r="N53" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O53" t="s">
         <v>28</v>
@@ -10929,7 +10926,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O54" t="s">
         <v>28</v>
@@ -10990,7 +10987,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O55" t="s">
         <v>26</v>
@@ -11053,7 +11050,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O56" t="s">
         <v>26</v>
@@ -11113,7 +11110,7 @@
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O57" t="s">
         <v>28</v>
@@ -11177,7 +11174,7 @@
         <v>0</v>
       </c>
       <c r="N58" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O58" t="s">
         <v>28</v>
@@ -11239,7 +11236,7 @@
         <v>0</v>
       </c>
       <c r="N59" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O59" t="s">
         <v>28</v>
@@ -11300,7 +11297,7 @@
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O60" t="s">
         <v>26</v>
@@ -11363,7 +11360,7 @@
         <v>0</v>
       </c>
       <c r="N61" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O61" t="s">
         <v>26</v>
@@ -11423,7 +11420,7 @@
         <v>0</v>
       </c>
       <c r="N62" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O62" t="s">
         <v>28</v>
@@ -11487,7 +11484,7 @@
         <v>0</v>
       </c>
       <c r="N63" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O63" t="s">
         <v>28</v>
@@ -11549,7 +11546,7 @@
         <v>0</v>
       </c>
       <c r="N64" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O64" t="s">
         <v>28</v>
@@ -11610,7 +11607,7 @@
         <v>0</v>
       </c>
       <c r="N65" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O65" t="s">
         <v>26</v>
@@ -11673,7 +11670,7 @@
         <v>0</v>
       </c>
       <c r="N66" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O66" t="s">
         <v>26</v>
@@ -11733,7 +11730,7 @@
         <v>0</v>
       </c>
       <c r="N67" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O67" t="s">
         <v>28</v>
@@ -11797,7 +11794,7 @@
         <v>0</v>
       </c>
       <c r="N68" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O68" t="s">
         <v>28</v>
@@ -11859,7 +11856,7 @@
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O69" t="s">
         <v>28</v>
@@ -11920,7 +11917,7 @@
         <v>0</v>
       </c>
       <c r="N70" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O70" t="s">
         <v>26</v>
@@ -11983,7 +11980,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O71" t="s">
         <v>26</v>
@@ -12043,7 +12040,7 @@
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O72" t="s">
         <v>28</v>
@@ -12107,7 +12104,7 @@
         <v>0</v>
       </c>
       <c r="N73" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O73" t="s">
         <v>28</v>
@@ -12169,7 +12166,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O74" t="s">
         <v>28</v>
@@ -12457,10 +12454,10 @@
         <v>0</v>
       </c>
       <c r="M79" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N79" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O79" t="s">
         <v>26</v>
@@ -12520,7 +12517,7 @@
         <v>0</v>
       </c>
       <c r="N80" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O80" t="s">
         <v>26</v>
@@ -12580,7 +12577,7 @@
         <v>0</v>
       </c>
       <c r="N81" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O81" t="s">
         <v>28</v>
@@ -12640,7 +12637,7 @@
         <v>0</v>
       </c>
       <c r="N82" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O82" t="s">
         <v>28</v>
@@ -12700,7 +12697,7 @@
         <v>0</v>
       </c>
       <c r="N83" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O83" t="s">
         <v>28</v>
@@ -12760,7 +12757,7 @@
         <v>0</v>
       </c>
       <c r="N84" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O84" t="s">
         <v>28</v>
@@ -12817,7 +12814,7 @@
         <v>0</v>
       </c>
       <c r="N85" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O85" t="s">
         <v>26</v>
@@ -12874,7 +12871,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O86" t="s">
         <v>26</v>
@@ -12931,7 +12928,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O87" t="s">
         <v>26</v>
@@ -12988,7 +12985,7 @@
         <v>0</v>
       </c>
       <c r="N88" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O88" t="s">
         <v>26</v>
@@ -13048,7 +13045,7 @@
         <v>0</v>
       </c>
       <c r="N89" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O89" t="s">
         <v>26</v>
@@ -13108,7 +13105,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O90" t="s">
         <v>26</v>
@@ -13168,7 +13165,7 @@
         <v>0</v>
       </c>
       <c r="N91" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O91" t="s">
         <v>26</v>
@@ -13228,7 +13225,7 @@
         <v>0</v>
       </c>
       <c r="N92" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O92" t="s">
         <v>26</v>
@@ -13288,7 +13285,7 @@
         <v>0</v>
       </c>
       <c r="N93" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O93" t="s">
         <v>26</v>
@@ -13348,7 +13345,7 @@
         <v>0</v>
       </c>
       <c r="N94" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O94" t="s">
         <v>26</v>
@@ -13408,7 +13405,7 @@
         <v>0</v>
       </c>
       <c r="N95" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O95" t="s">
         <v>26</v>
@@ -13468,7 +13465,7 @@
         <v>0</v>
       </c>
       <c r="N96" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O96" t="s">
         <v>26</v>
@@ -13528,7 +13525,7 @@
         <v>0</v>
       </c>
       <c r="N97" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O97" t="s">
         <v>26</v>
@@ -13588,7 +13585,7 @@
         <v>0</v>
       </c>
       <c r="N98" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O98" t="s">
         <v>26</v>
@@ -13648,7 +13645,7 @@
         <v>0</v>
       </c>
       <c r="N99" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O99" t="s">
         <v>26</v>
@@ -13708,7 +13705,7 @@
         <v>0</v>
       </c>
       <c r="N100" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O100" t="s">
         <v>26</v>
@@ -13768,7 +13765,7 @@
         <v>0</v>
       </c>
       <c r="N101" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O101" t="s">
         <v>26</v>
@@ -13828,7 +13825,7 @@
         <v>0</v>
       </c>
       <c r="N102" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O102" t="s">
         <v>26</v>
@@ -13888,7 +13885,7 @@
         <v>0</v>
       </c>
       <c r="N103" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O103" t="s">
         <v>26</v>
@@ -13948,7 +13945,7 @@
         <v>0</v>
       </c>
       <c r="N104" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O104" t="s">
         <v>26</v>
@@ -14008,7 +14005,7 @@
         <v>0</v>
       </c>
       <c r="N105" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O105" t="s">
         <v>26</v>
@@ -14068,7 +14065,7 @@
         <v>0</v>
       </c>
       <c r="N106" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O106" t="s">
         <v>26</v>
@@ -14128,7 +14125,7 @@
         <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O107" t="s">
         <v>26</v>
@@ -14188,7 +14185,7 @@
         <v>0</v>
       </c>
       <c r="N108" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O108" t="s">
         <v>26</v>
@@ -14248,7 +14245,7 @@
         <v>0</v>
       </c>
       <c r="N109" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O109" t="s">
         <v>26</v>
@@ -14308,7 +14305,7 @@
         <v>0</v>
       </c>
       <c r="N110" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O110" t="s">
         <v>26</v>
@@ -14368,7 +14365,7 @@
         <v>0</v>
       </c>
       <c r="N111" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O111" t="s">
         <v>26</v>
@@ -14428,7 +14425,7 @@
         <v>0</v>
       </c>
       <c r="N112" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O112" t="s">
         <v>26</v>
@@ -14488,7 +14485,7 @@
         <v>0</v>
       </c>
       <c r="N113" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O113" t="s">
         <v>26</v>
@@ -14548,7 +14545,7 @@
         <v>0</v>
       </c>
       <c r="N114" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O114" t="s">
         <v>26</v>
@@ -14608,7 +14605,7 @@
         <v>0</v>
       </c>
       <c r="N115" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O115" t="s">
         <v>26</v>
@@ -14668,7 +14665,7 @@
         <v>0</v>
       </c>
       <c r="N116" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O116" t="s">
         <v>26</v>
@@ -14728,7 +14725,7 @@
         <v>0</v>
       </c>
       <c r="N117" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O117" t="s">
         <v>26</v>
@@ -14788,7 +14785,7 @@
         <v>0</v>
       </c>
       <c r="N118" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O118" t="s">
         <v>26</v>
@@ -14848,7 +14845,7 @@
         <v>0</v>
       </c>
       <c r="N119" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O119" t="s">
         <v>26</v>
@@ -14908,7 +14905,7 @@
         <v>0</v>
       </c>
       <c r="N120" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O120" t="s">
         <v>26</v>
@@ -14968,7 +14965,7 @@
         <v>0</v>
       </c>
       <c r="N121" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O121" t="s">
         <v>26</v>
@@ -15028,7 +15025,7 @@
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O122" t="s">
         <v>26</v>
@@ -15088,7 +15085,7 @@
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O123" t="s">
         <v>26</v>
@@ -15945,10 +15942,10 @@
         <v>0</v>
       </c>
       <c r="M138" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N138" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O138" t="s">
         <v>26</v>
@@ -16008,7 +16005,7 @@
         <v>0</v>
       </c>
       <c r="N139" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O139" t="s">
         <v>26</v>
@@ -16068,7 +16065,7 @@
         <v>0</v>
       </c>
       <c r="N140" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O140" t="s">
         <v>28</v>
@@ -16128,7 +16125,7 @@
         <v>0</v>
       </c>
       <c r="N141" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O141" t="s">
         <v>28</v>
@@ -16188,7 +16185,7 @@
         <v>0</v>
       </c>
       <c r="N142" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O142" t="s">
         <v>28</v>
@@ -16248,7 +16245,7 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O143" t="s">
         <v>28</v>
@@ -16305,7 +16302,7 @@
         <v>0</v>
       </c>
       <c r="N144" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O144" t="s">
         <v>26</v>
@@ -16362,7 +16359,7 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O145" t="s">
         <v>26</v>
@@ -16419,7 +16416,7 @@
         <v>0</v>
       </c>
       <c r="N146" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O146" t="s">
         <v>26</v>
@@ -16476,7 +16473,7 @@
         <v>0</v>
       </c>
       <c r="N147" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O147" t="s">
         <v>26</v>
@@ -16536,7 +16533,7 @@
         <v>0</v>
       </c>
       <c r="N148" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O148" t="s">
         <v>26</v>
@@ -16596,7 +16593,7 @@
         <v>0</v>
       </c>
       <c r="N149" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O149" t="s">
         <v>26</v>
@@ -16656,7 +16653,7 @@
         <v>0</v>
       </c>
       <c r="N150" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O150" t="s">
         <v>26</v>
@@ -16716,7 +16713,7 @@
         <v>0</v>
       </c>
       <c r="N151" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O151" t="s">
         <v>26</v>
@@ -16776,7 +16773,7 @@
         <v>0</v>
       </c>
       <c r="N152" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O152" t="s">
         <v>26</v>
@@ -16836,7 +16833,7 @@
         <v>0</v>
       </c>
       <c r="N153" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O153" t="s">
         <v>26</v>
@@ -16896,7 +16893,7 @@
         <v>0</v>
       </c>
       <c r="N154" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O154" t="s">
         <v>26</v>
@@ -16956,7 +16953,7 @@
         <v>0</v>
       </c>
       <c r="N155" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O155" t="s">
         <v>26</v>
@@ -17016,7 +17013,7 @@
         <v>0</v>
       </c>
       <c r="N156" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O156" t="s">
         <v>26</v>
@@ -17076,7 +17073,7 @@
         <v>0</v>
       </c>
       <c r="N157" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O157" t="s">
         <v>26</v>
@@ -17136,7 +17133,7 @@
         <v>0</v>
       </c>
       <c r="N158" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O158" t="s">
         <v>26</v>
@@ -17196,7 +17193,7 @@
         <v>0</v>
       </c>
       <c r="N159" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O159" t="s">
         <v>26</v>
@@ -17256,7 +17253,7 @@
         <v>0</v>
       </c>
       <c r="N160" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O160" t="s">
         <v>26</v>
@@ -17316,7 +17313,7 @@
         <v>0</v>
       </c>
       <c r="N161" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O161" t="s">
         <v>26</v>
@@ -17376,7 +17373,7 @@
         <v>0</v>
       </c>
       <c r="N162" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O162" t="s">
         <v>26</v>
@@ -17436,7 +17433,7 @@
         <v>0</v>
       </c>
       <c r="N163" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O163" t="s">
         <v>26</v>
@@ -17496,7 +17493,7 @@
         <v>0</v>
       </c>
       <c r="N164" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O164" t="s">
         <v>26</v>
@@ -17556,7 +17553,7 @@
         <v>0</v>
       </c>
       <c r="N165" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O165" t="s">
         <v>26</v>
@@ -17616,7 +17613,7 @@
         <v>0</v>
       </c>
       <c r="N166" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O166" t="s">
         <v>26</v>
@@ -17676,7 +17673,7 @@
         <v>0</v>
       </c>
       <c r="N167" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O167" t="s">
         <v>26</v>
@@ -17904,10 +17901,10 @@
         <v>0</v>
       </c>
       <c r="M171" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N171" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O171" t="s">
         <v>26</v>
@@ -17967,7 +17964,7 @@
         <v>0</v>
       </c>
       <c r="N172" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O172" t="s">
         <v>26</v>
@@ -18027,7 +18024,7 @@
         <v>0</v>
       </c>
       <c r="N173" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O173" t="s">
         <v>28</v>
@@ -18087,7 +18084,7 @@
         <v>0</v>
       </c>
       <c r="N174" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O174" t="s">
         <v>28</v>
@@ -18147,7 +18144,7 @@
         <v>0</v>
       </c>
       <c r="N175" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O175" t="s">
         <v>28</v>
@@ -18207,7 +18204,7 @@
         <v>0</v>
       </c>
       <c r="N176" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O176" t="s">
         <v>28</v>
@@ -18264,7 +18261,7 @@
         <v>0</v>
       </c>
       <c r="N177" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O177" t="s">
         <v>26</v>
@@ -18321,7 +18318,7 @@
         <v>0</v>
       </c>
       <c r="N178" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O178" t="s">
         <v>26</v>
@@ -18378,7 +18375,7 @@
         <v>0</v>
       </c>
       <c r="N179" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O179" t="s">
         <v>26</v>
@@ -18435,7 +18432,7 @@
         <v>0</v>
       </c>
       <c r="N180" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O180" t="s">
         <v>26</v>
@@ -18495,7 +18492,7 @@
         <v>0</v>
       </c>
       <c r="N181" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O181" t="s">
         <v>26</v>
@@ -18555,7 +18552,7 @@
         <v>0</v>
       </c>
       <c r="N182" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O182" t="s">
         <v>26</v>
@@ -18615,7 +18612,7 @@
         <v>0</v>
       </c>
       <c r="N183" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O183" t="s">
         <v>26</v>
@@ -18675,7 +18672,7 @@
         <v>0</v>
       </c>
       <c r="N184" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O184" t="s">
         <v>26</v>
@@ -18735,7 +18732,7 @@
         <v>0</v>
       </c>
       <c r="N185" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O185" t="s">
         <v>26</v>
@@ -18789,10 +18786,10 @@
         <v>0</v>
       </c>
       <c r="M186" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="N186" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O186" t="s">
         <v>26</v>
@@ -18850,7 +18847,7 @@
         <v>0</v>
       </c>
       <c r="N187" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O187" t="s">
         <v>208</v>
@@ -18910,7 +18907,7 @@
         <v>0</v>
       </c>
       <c r="N188" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O188" t="s">
         <v>208</v>
@@ -19044,7 +19041,7 @@
     </row>
     <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B191">
         <v>6</v>
@@ -19145,7 +19142,7 @@
         <v>26</v>
       </c>
       <c r="P192" s="6" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="Q192">
         <v>2</v>
@@ -19984,7 +19981,7 @@
         <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="Q12">
         <v>3</v>
@@ -20042,7 +20039,7 @@
         <v>28</v>
       </c>
       <c r="P13" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -20740,7 +20737,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -21357,10 +21354,10 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="N36" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O36" t="s">
         <v>26</v>
@@ -21420,7 +21417,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O37" t="s">
         <v>26</v>
@@ -21480,7 +21477,7 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -21537,7 +21534,7 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O39" t="s">
         <v>26</v>
@@ -21597,7 +21594,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O40" t="s">
         <v>28</v>
@@ -21658,7 +21655,7 @@
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>28</v>
@@ -21720,7 +21717,7 @@
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>28</v>
@@ -21778,7 +21775,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O43" t="s">
         <v>26</v>
@@ -21834,7 +21831,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O44" t="s">
         <v>26</v>
@@ -21894,7 +21891,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O45" t="s">
         <v>26</v>
@@ -21957,7 +21954,7 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O46" t="s">
         <v>26</v>
@@ -22017,7 +22014,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O47" t="s">
         <v>28</v>
@@ -22081,7 +22078,7 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O48" t="s">
         <v>28</v>
@@ -22143,7 +22140,7 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O49" t="s">
         <v>28</v>
@@ -22204,7 +22201,7 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O50" t="s">
         <v>26</v>
@@ -22267,7 +22264,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O51" t="s">
         <v>26</v>
@@ -22327,7 +22324,7 @@
         <v>0</v>
       </c>
       <c r="N52" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O52" t="s">
         <v>28</v>
@@ -22391,7 +22388,7 @@
         <v>0</v>
       </c>
       <c r="N53" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O53" t="s">
         <v>28</v>
@@ -22453,7 +22450,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O54" t="s">
         <v>28</v>
@@ -22514,7 +22511,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O55" t="s">
         <v>26</v>
@@ -22577,7 +22574,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O56" t="s">
         <v>26</v>
@@ -22637,7 +22634,7 @@
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O57" t="s">
         <v>28</v>
@@ -22701,7 +22698,7 @@
         <v>0</v>
       </c>
       <c r="N58" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O58" t="s">
         <v>28</v>
@@ -22763,7 +22760,7 @@
         <v>0</v>
       </c>
       <c r="N59" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O59" t="s">
         <v>28</v>
@@ -22824,7 +22821,7 @@
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O60" t="s">
         <v>26</v>
@@ -22887,7 +22884,7 @@
         <v>0</v>
       </c>
       <c r="N61" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O61" t="s">
         <v>26</v>
@@ -22947,7 +22944,7 @@
         <v>0</v>
       </c>
       <c r="N62" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O62" t="s">
         <v>28</v>
@@ -23011,7 +23008,7 @@
         <v>0</v>
       </c>
       <c r="N63" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O63" t="s">
         <v>28</v>
@@ -23073,7 +23070,7 @@
         <v>0</v>
       </c>
       <c r="N64" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O64" t="s">
         <v>28</v>
@@ -23134,7 +23131,7 @@
         <v>0</v>
       </c>
       <c r="N65" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O65" t="s">
         <v>26</v>
@@ -23197,7 +23194,7 @@
         <v>0</v>
       </c>
       <c r="N66" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O66" t="s">
         <v>26</v>
@@ -23257,7 +23254,7 @@
         <v>0</v>
       </c>
       <c r="N67" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O67" t="s">
         <v>28</v>
@@ -23321,7 +23318,7 @@
         <v>0</v>
       </c>
       <c r="N68" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O68" t="s">
         <v>28</v>
@@ -23383,7 +23380,7 @@
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O69" t="s">
         <v>28</v>
@@ -23444,7 +23441,7 @@
         <v>0</v>
       </c>
       <c r="N70" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O70" t="s">
         <v>26</v>
@@ -23507,7 +23504,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O71" t="s">
         <v>26</v>
@@ -23567,7 +23564,7 @@
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O72" t="s">
         <v>28</v>
@@ -23631,7 +23628,7 @@
         <v>0</v>
       </c>
       <c r="N73" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O73" t="s">
         <v>28</v>
@@ -23693,7 +23690,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O74" t="s">
         <v>28</v>
@@ -23981,10 +23978,10 @@
         <v>0</v>
       </c>
       <c r="M79" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N79" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O79" t="s">
         <v>26</v>
@@ -24044,7 +24041,7 @@
         <v>0</v>
       </c>
       <c r="N80" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O80" t="s">
         <v>26</v>
@@ -24104,7 +24101,7 @@
         <v>0</v>
       </c>
       <c r="N81" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O81" t="s">
         <v>28</v>
@@ -24164,7 +24161,7 @@
         <v>0</v>
       </c>
       <c r="N82" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O82" t="s">
         <v>28</v>
@@ -24224,7 +24221,7 @@
         <v>0</v>
       </c>
       <c r="N83" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O83" t="s">
         <v>28</v>
@@ -24284,7 +24281,7 @@
         <v>0</v>
       </c>
       <c r="N84" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O84" t="s">
         <v>28</v>
@@ -24341,7 +24338,7 @@
         <v>0</v>
       </c>
       <c r="N85" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O85" t="s">
         <v>26</v>
@@ -24398,7 +24395,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O86" t="s">
         <v>26</v>
@@ -24455,7 +24452,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O87" t="s">
         <v>26</v>
@@ -24512,7 +24509,7 @@
         <v>0</v>
       </c>
       <c r="N88" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O88" t="s">
         <v>26</v>
@@ -24572,7 +24569,7 @@
         <v>0</v>
       </c>
       <c r="N89" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O89" t="s">
         <v>26</v>
@@ -24632,7 +24629,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O90" t="s">
         <v>26</v>
@@ -24692,7 +24689,7 @@
         <v>0</v>
       </c>
       <c r="N91" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O91" t="s">
         <v>26</v>
@@ -24752,7 +24749,7 @@
         <v>0</v>
       </c>
       <c r="N92" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O92" t="s">
         <v>26</v>
@@ -24812,7 +24809,7 @@
         <v>0</v>
       </c>
       <c r="N93" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O93" t="s">
         <v>26</v>
@@ -24872,7 +24869,7 @@
         <v>0</v>
       </c>
       <c r="N94" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O94" t="s">
         <v>26</v>
@@ -24932,7 +24929,7 @@
         <v>0</v>
       </c>
       <c r="N95" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O95" t="s">
         <v>26</v>
@@ -24992,7 +24989,7 @@
         <v>0</v>
       </c>
       <c r="N96" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O96" t="s">
         <v>26</v>
@@ -25052,7 +25049,7 @@
         <v>0</v>
       </c>
       <c r="N97" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O97" t="s">
         <v>26</v>
@@ -25112,7 +25109,7 @@
         <v>0</v>
       </c>
       <c r="N98" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O98" t="s">
         <v>26</v>
@@ -25172,7 +25169,7 @@
         <v>0</v>
       </c>
       <c r="N99" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O99" t="s">
         <v>26</v>
@@ -25232,7 +25229,7 @@
         <v>0</v>
       </c>
       <c r="N100" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O100" t="s">
         <v>26</v>
@@ -25292,7 +25289,7 @@
         <v>0</v>
       </c>
       <c r="N101" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O101" t="s">
         <v>26</v>
@@ -25352,7 +25349,7 @@
         <v>0</v>
       </c>
       <c r="N102" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O102" t="s">
         <v>26</v>
@@ -25412,7 +25409,7 @@
         <v>0</v>
       </c>
       <c r="N103" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O103" t="s">
         <v>26</v>
@@ -25472,7 +25469,7 @@
         <v>0</v>
       </c>
       <c r="N104" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O104" t="s">
         <v>26</v>
@@ -25532,7 +25529,7 @@
         <v>0</v>
       </c>
       <c r="N105" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O105" t="s">
         <v>26</v>
@@ -25592,7 +25589,7 @@
         <v>0</v>
       </c>
       <c r="N106" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O106" t="s">
         <v>26</v>
@@ -25652,7 +25649,7 @@
         <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O107" t="s">
         <v>26</v>
@@ -25712,7 +25709,7 @@
         <v>0</v>
       </c>
       <c r="N108" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O108" t="s">
         <v>26</v>
@@ -25772,7 +25769,7 @@
         <v>0</v>
       </c>
       <c r="N109" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O109" t="s">
         <v>26</v>
@@ -25832,7 +25829,7 @@
         <v>0</v>
       </c>
       <c r="N110" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O110" t="s">
         <v>26</v>
@@ -25892,7 +25889,7 @@
         <v>0</v>
       </c>
       <c r="N111" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O111" t="s">
         <v>26</v>
@@ -25952,7 +25949,7 @@
         <v>0</v>
       </c>
       <c r="N112" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O112" t="s">
         <v>26</v>
@@ -26012,7 +26009,7 @@
         <v>0</v>
       </c>
       <c r="N113" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O113" t="s">
         <v>26</v>
@@ -26072,7 +26069,7 @@
         <v>0</v>
       </c>
       <c r="N114" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O114" t="s">
         <v>26</v>
@@ -26132,7 +26129,7 @@
         <v>0</v>
       </c>
       <c r="N115" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O115" t="s">
         <v>26</v>
@@ -26192,7 +26189,7 @@
         <v>0</v>
       </c>
       <c r="N116" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O116" t="s">
         <v>26</v>
@@ -26252,7 +26249,7 @@
         <v>0</v>
       </c>
       <c r="N117" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O117" t="s">
         <v>26</v>
@@ -26312,7 +26309,7 @@
         <v>0</v>
       </c>
       <c r="N118" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O118" t="s">
         <v>26</v>
@@ -26372,7 +26369,7 @@
         <v>0</v>
       </c>
       <c r="N119" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O119" t="s">
         <v>26</v>
@@ -26432,7 +26429,7 @@
         <v>0</v>
       </c>
       <c r="N120" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O120" t="s">
         <v>26</v>
@@ -26492,7 +26489,7 @@
         <v>0</v>
       </c>
       <c r="N121" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O121" t="s">
         <v>26</v>
@@ -26552,7 +26549,7 @@
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O122" t="s">
         <v>26</v>
@@ -26612,7 +26609,7 @@
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O123" t="s">
         <v>26</v>
@@ -27469,10 +27466,10 @@
         <v>0</v>
       </c>
       <c r="M138" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N138" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O138" t="s">
         <v>26</v>
@@ -27532,7 +27529,7 @@
         <v>0</v>
       </c>
       <c r="N139" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O139" t="s">
         <v>26</v>
@@ -27592,7 +27589,7 @@
         <v>0</v>
       </c>
       <c r="N140" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O140" t="s">
         <v>28</v>
@@ -27652,7 +27649,7 @@
         <v>0</v>
       </c>
       <c r="N141" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O141" t="s">
         <v>28</v>
@@ -27712,7 +27709,7 @@
         <v>0</v>
       </c>
       <c r="N142" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O142" t="s">
         <v>28</v>
@@ -27772,7 +27769,7 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O143" t="s">
         <v>28</v>
@@ -27829,7 +27826,7 @@
         <v>0</v>
       </c>
       <c r="N144" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O144" t="s">
         <v>26</v>
@@ -27886,7 +27883,7 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O145" t="s">
         <v>26</v>
@@ -27943,7 +27940,7 @@
         <v>0</v>
       </c>
       <c r="N146" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O146" t="s">
         <v>26</v>
@@ -28000,7 +27997,7 @@
         <v>0</v>
       </c>
       <c r="N147" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O147" t="s">
         <v>26</v>
@@ -28060,7 +28057,7 @@
         <v>0</v>
       </c>
       <c r="N148" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O148" t="s">
         <v>26</v>
@@ -28120,7 +28117,7 @@
         <v>0</v>
       </c>
       <c r="N149" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O149" t="s">
         <v>26</v>
@@ -28180,7 +28177,7 @@
         <v>0</v>
       </c>
       <c r="N150" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O150" t="s">
         <v>26</v>
@@ -28240,7 +28237,7 @@
         <v>0</v>
       </c>
       <c r="N151" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O151" t="s">
         <v>26</v>
@@ -28300,7 +28297,7 @@
         <v>0</v>
       </c>
       <c r="N152" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O152" t="s">
         <v>26</v>
@@ -28360,7 +28357,7 @@
         <v>0</v>
       </c>
       <c r="N153" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O153" t="s">
         <v>26</v>
@@ -28420,7 +28417,7 @@
         <v>0</v>
       </c>
       <c r="N154" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O154" t="s">
         <v>26</v>
@@ -28480,7 +28477,7 @@
         <v>0</v>
       </c>
       <c r="N155" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O155" t="s">
         <v>26</v>
@@ -28540,7 +28537,7 @@
         <v>0</v>
       </c>
       <c r="N156" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O156" t="s">
         <v>26</v>
@@ -28600,7 +28597,7 @@
         <v>0</v>
       </c>
       <c r="N157" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O157" t="s">
         <v>26</v>
@@ -28660,7 +28657,7 @@
         <v>0</v>
       </c>
       <c r="N158" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O158" t="s">
         <v>26</v>
@@ -28720,7 +28717,7 @@
         <v>0</v>
       </c>
       <c r="N159" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O159" t="s">
         <v>26</v>
@@ -28780,7 +28777,7 @@
         <v>0</v>
       </c>
       <c r="N160" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O160" t="s">
         <v>26</v>
@@ -28840,7 +28837,7 @@
         <v>0</v>
       </c>
       <c r="N161" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O161" t="s">
         <v>26</v>
@@ -28900,7 +28897,7 @@
         <v>0</v>
       </c>
       <c r="N162" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O162" t="s">
         <v>26</v>
@@ -28960,7 +28957,7 @@
         <v>0</v>
       </c>
       <c r="N163" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O163" t="s">
         <v>26</v>
@@ -29020,7 +29017,7 @@
         <v>0</v>
       </c>
       <c r="N164" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O164" t="s">
         <v>26</v>
@@ -29080,7 +29077,7 @@
         <v>0</v>
       </c>
       <c r="N165" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O165" t="s">
         <v>26</v>
@@ -29140,7 +29137,7 @@
         <v>0</v>
       </c>
       <c r="N166" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O166" t="s">
         <v>26</v>
@@ -29200,7 +29197,7 @@
         <v>0</v>
       </c>
       <c r="N167" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O167" t="s">
         <v>26</v>
@@ -29428,10 +29425,10 @@
         <v>0</v>
       </c>
       <c r="M171" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N171" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O171" t="s">
         <v>26</v>
@@ -29491,7 +29488,7 @@
         <v>0</v>
       </c>
       <c r="N172" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O172" t="s">
         <v>26</v>
@@ -29551,7 +29548,7 @@
         <v>0</v>
       </c>
       <c r="N173" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O173" t="s">
         <v>28</v>
@@ -29611,7 +29608,7 @@
         <v>0</v>
       </c>
       <c r="N174" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O174" t="s">
         <v>28</v>
@@ -29671,7 +29668,7 @@
         <v>0</v>
       </c>
       <c r="N175" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O175" t="s">
         <v>28</v>
@@ -29731,7 +29728,7 @@
         <v>0</v>
       </c>
       <c r="N176" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O176" t="s">
         <v>28</v>
@@ -29788,7 +29785,7 @@
         <v>0</v>
       </c>
       <c r="N177" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O177" t="s">
         <v>26</v>
@@ -29845,7 +29842,7 @@
         <v>0</v>
       </c>
       <c r="N178" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O178" t="s">
         <v>26</v>
@@ -29902,7 +29899,7 @@
         <v>0</v>
       </c>
       <c r="N179" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O179" t="s">
         <v>26</v>
@@ -29959,7 +29956,7 @@
         <v>0</v>
       </c>
       <c r="N180" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O180" t="s">
         <v>26</v>
@@ -30019,7 +30016,7 @@
         <v>0</v>
       </c>
       <c r="N181" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O181" t="s">
         <v>26</v>
@@ -30079,7 +30076,7 @@
         <v>0</v>
       </c>
       <c r="N182" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O182" t="s">
         <v>26</v>
@@ -30139,7 +30136,7 @@
         <v>0</v>
       </c>
       <c r="N183" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O183" t="s">
         <v>26</v>
@@ -30199,7 +30196,7 @@
         <v>0</v>
       </c>
       <c r="N184" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O184" t="s">
         <v>26</v>
@@ -30259,7 +30256,7 @@
         <v>0</v>
       </c>
       <c r="N185" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="O185" t="s">
         <v>26</v>
@@ -30313,10 +30310,10 @@
         <v>0</v>
       </c>
       <c r="M186" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="N186" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O186" t="s">
         <v>26</v>
@@ -30374,7 +30371,7 @@
         <v>0</v>
       </c>
       <c r="N187" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O187" t="s">
         <v>208</v>
@@ -30434,7 +30431,7 @@
         <v>0</v>
       </c>
       <c r="N188" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="O188" t="s">
         <v>208</v>
@@ -30568,7 +30565,7 @@
     </row>
     <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B191">
         <v>8</v>
@@ -30669,7 +30666,7 @@
         <v>26</v>
       </c>
       <c r="P192" s="6" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="Q192">
         <v>2</v>
@@ -30815,11 +30812,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H89" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="S167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J90" sqref="J90"/>
+      <selection pane="bottomRight" activeCell="T168" sqref="T168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30970,7 +30967,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="C3" s="53">
         <v>1</v>
@@ -31110,16 +31107,16 @@
         <v>967</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>1309</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>440</v>
@@ -31138,7 +31135,7 @@
         <v>787</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="Q5" s="11" t="s">
         <v>465</v>
@@ -31147,7 +31144,7 @@
         <v>1672</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>1293</v>
@@ -33364,7 +33361,7 @@
         <v>487</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="K64" s="22" t="s">
         <v>1383</v>
@@ -33426,7 +33423,7 @@
         <v>1189</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="K65" s="22" t="s">
         <v>1384</v>
@@ -33550,7 +33547,7 @@
         <v>1191</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="K67" s="22" t="s">
         <v>1386</v>
@@ -34111,7 +34108,7 @@
         <v>1572</v>
       </c>
       <c r="K76" s="22" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="L76" s="22"/>
       <c r="M76" s="22" t="s">
@@ -34149,56 +34146,56 @@
         <v>578</v>
       </c>
       <c r="C77" s="10" t="s">
+        <v>1859</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>1860</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="E77" s="9" t="s">
         <v>1861</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="F77" s="9" t="s">
         <v>1862</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="G77" s="10" t="s">
         <v>1863</v>
       </c>
-      <c r="G77" s="10" t="s">
+      <c r="H77" s="9" t="s">
         <v>1864</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="I77" s="22" t="s">
         <v>1865</v>
       </c>
-      <c r="I77" s="22" t="s">
+      <c r="J77" s="9" t="s">
         <v>1866</v>
       </c>
-      <c r="J77" s="9" t="s">
+      <c r="K77" s="22" t="s">
         <v>1867</v>
-      </c>
-      <c r="K77" s="22" t="s">
-        <v>1868</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22" t="s">
+        <v>1868</v>
+      </c>
+      <c r="N77" s="9" t="s">
         <v>1869</v>
       </c>
-      <c r="N77" s="9" t="s">
+      <c r="O77" s="11" t="s">
         <v>1870</v>
       </c>
-      <c r="O77" s="11" t="s">
+      <c r="P77" s="9" t="s">
         <v>1871</v>
       </c>
-      <c r="P77" s="9" t="s">
+      <c r="Q77" s="9" t="s">
         <v>1872</v>
       </c>
-      <c r="Q77" s="9" t="s">
+      <c r="R77" s="9" t="s">
         <v>1873</v>
-      </c>
-      <c r="R77" s="9" t="s">
-        <v>1874</v>
       </c>
       <c r="S77" s="9" t="s">
         <v>1738</v>
       </c>
       <c r="T77" s="9" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="U77" s="9"/>
       <c r="V77" s="9"/>
@@ -34211,56 +34208,56 @@
         <v>579</v>
       </c>
       <c r="C78" s="10" t="s">
+        <v>1875</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>1876</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="E78" s="9" t="s">
         <v>1877</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="F78" s="9" t="s">
         <v>1878</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="G78" s="10" t="s">
         <v>1879</v>
       </c>
-      <c r="G78" s="10" t="s">
+      <c r="H78" s="9" t="s">
         <v>1880</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="I78" s="22" t="s">
         <v>1881</v>
       </c>
-      <c r="I78" s="22" t="s">
+      <c r="J78" s="9" t="s">
         <v>1882</v>
       </c>
-      <c r="J78" s="9" t="s">
+      <c r="K78" s="22" t="s">
         <v>1883</v>
-      </c>
-      <c r="K78" s="22" t="s">
-        <v>1884</v>
       </c>
       <c r="L78" s="22"/>
       <c r="M78" s="22" t="s">
+        <v>1884</v>
+      </c>
+      <c r="N78" s="9" t="s">
         <v>1885</v>
       </c>
-      <c r="N78" s="9" t="s">
+      <c r="O78" s="11" t="s">
         <v>1886</v>
       </c>
-      <c r="O78" s="11" t="s">
+      <c r="P78" s="9" t="s">
         <v>1887</v>
       </c>
-      <c r="P78" s="9" t="s">
+      <c r="Q78" s="9" t="s">
         <v>1888</v>
       </c>
-      <c r="Q78" s="9" t="s">
+      <c r="R78" s="9" t="s">
         <v>1889</v>
-      </c>
-      <c r="R78" s="9" t="s">
-        <v>1890</v>
       </c>
       <c r="S78" s="9" t="s">
         <v>1739</v>
       </c>
       <c r="T78" s="9" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="U78" s="9"/>
       <c r="V78" s="9"/>
@@ -34273,56 +34270,56 @@
         <v>577</v>
       </c>
       <c r="C79" s="10" t="s">
+        <v>1891</v>
+      </c>
+      <c r="D79" s="9" t="s">
         <v>1892</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="E79" s="9" t="s">
         <v>1893</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="F79" s="9" t="s">
         <v>1894</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="G79" s="10" t="s">
         <v>1895</v>
       </c>
-      <c r="G79" s="10" t="s">
+      <c r="H79" s="9" t="s">
         <v>1896</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="I79" s="22" t="s">
         <v>1897</v>
       </c>
-      <c r="I79" s="22" t="s">
+      <c r="J79" s="9" t="s">
         <v>1898</v>
       </c>
-      <c r="J79" s="9" t="s">
+      <c r="K79" s="22" t="s">
         <v>1899</v>
-      </c>
-      <c r="K79" s="22" t="s">
-        <v>1900</v>
       </c>
       <c r="L79" s="22"/>
       <c r="M79" s="22" t="s">
+        <v>1900</v>
+      </c>
+      <c r="N79" s="9" t="s">
         <v>1901</v>
       </c>
-      <c r="N79" s="9" t="s">
+      <c r="O79" s="9" t="s">
         <v>1902</v>
       </c>
-      <c r="O79" s="9" t="s">
+      <c r="P79" s="9" t="s">
         <v>1903</v>
       </c>
-      <c r="P79" s="9" t="s">
+      <c r="Q79" s="9" t="s">
         <v>1904</v>
       </c>
-      <c r="Q79" s="9" t="s">
+      <c r="R79" s="9" t="s">
         <v>1905</v>
-      </c>
-      <c r="R79" s="9" t="s">
-        <v>1906</v>
       </c>
       <c r="S79" s="9" t="s">
         <v>1737</v>
       </c>
       <c r="T79" s="9" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="U79" s="9"/>
       <c r="V79" s="9"/>
@@ -34828,7 +34825,7 @@
         <v>146</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>1598</v>
@@ -34877,7 +34874,7 @@
         <v>1690</v>
       </c>
       <c r="S88" s="11" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="T88" s="11" t="s">
         <v>1606</v>
@@ -34893,56 +34890,56 @@
         <v>182</v>
       </c>
       <c r="C89" s="12" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>1994</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>1995</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>1996</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>1997</v>
+      </c>
+      <c r="I89" s="22" t="s">
+        <v>1998</v>
+      </c>
+      <c r="J89" s="11" t="s">
         <v>1990</v>
       </c>
-      <c r="D89" s="11" t="s">
-        <v>1994</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>1995</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>1996</v>
-      </c>
-      <c r="G89" s="12" t="s">
-        <v>1997</v>
-      </c>
-      <c r="H89" s="11" t="s">
-        <v>1998</v>
-      </c>
-      <c r="I89" s="22" t="s">
-        <v>1999</v>
-      </c>
-      <c r="J89" s="11" t="s">
+      <c r="K89" s="22" t="s">
         <v>1991</v>
-      </c>
-      <c r="K89" s="22" t="s">
-        <v>1992</v>
       </c>
       <c r="L89" s="22"/>
       <c r="M89" s="22" t="s">
+        <v>2000</v>
+      </c>
+      <c r="N89" s="11" t="s">
+        <v>1992</v>
+      </c>
+      <c r="O89" s="11" t="s">
         <v>2001</v>
       </c>
-      <c r="N89" s="11" t="s">
-        <v>1993</v>
-      </c>
-      <c r="O89" s="11" t="s">
+      <c r="P89" s="11" t="s">
         <v>2002</v>
       </c>
-      <c r="P89" s="11" t="s">
+      <c r="Q89" s="11" t="s">
         <v>2003</v>
       </c>
-      <c r="Q89" s="11" t="s">
+      <c r="R89" s="11" t="s">
         <v>2004</v>
       </c>
-      <c r="R89" s="11" t="s">
+      <c r="S89" s="11" t="s">
+        <v>2006</v>
+      </c>
+      <c r="T89" s="11" t="s">
         <v>2005</v>
-      </c>
-      <c r="S89" s="11" t="s">
-        <v>2007</v>
-      </c>
-      <c r="T89" s="11" t="s">
-        <v>2006</v>
       </c>
       <c r="U89" s="11"/>
       <c r="V89" s="11"/>
@@ -34976,7 +34973,7 @@
         <v>1544</v>
       </c>
       <c r="J90" s="11" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="K90" s="22" t="s">
         <v>1448</v>
@@ -34986,7 +34983,7 @@
         <v>629</v>
       </c>
       <c r="N90" s="11" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="O90" s="11" t="s">
         <v>796</v>
@@ -35001,7 +34998,7 @@
         <v>1684</v>
       </c>
       <c r="S90" s="11" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="T90" s="11" t="s">
         <v>1294</v>
@@ -35249,7 +35246,7 @@
         <v>1687</v>
       </c>
       <c r="S94" s="11" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="T94" s="11" t="s">
         <v>1304</v>
@@ -35451,56 +35448,56 @@
         <v>40</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="J98" s="11" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="K98" s="22" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="L98" s="22"/>
       <c r="M98" s="22" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="N98" s="11" t="s">
+        <v>1942</v>
+      </c>
+      <c r="O98" s="11" t="s">
         <v>1943</v>
       </c>
-      <c r="O98" s="11" t="s">
+      <c r="P98" s="11" t="s">
         <v>1944</v>
       </c>
-      <c r="P98" s="11" t="s">
+      <c r="Q98" s="11" t="s">
         <v>1945</v>
-      </c>
-      <c r="Q98" s="11" t="s">
-        <v>1946</v>
       </c>
       <c r="R98" s="11" t="s">
         <v>1689</v>
       </c>
       <c r="S98" s="11" t="s">
+        <v>1946</v>
+      </c>
+      <c r="T98" s="11" t="s">
         <v>1947</v>
-      </c>
-      <c r="T98" s="11" t="s">
-        <v>1948</v>
       </c>
       <c r="U98" s="11"/>
       <c r="V98" s="11"/>
@@ -35745,7 +35742,7 @@
         <v>373</v>
       </c>
       <c r="S102" s="11" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="T102" s="11" t="s">
         <v>1264</v>
@@ -35782,7 +35779,7 @@
         <v>1208</v>
       </c>
       <c r="J103" s="11" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="K103" s="22" t="s">
         <v>1412</v>
@@ -35792,7 +35789,7 @@
         <v>639</v>
       </c>
       <c r="N103" s="11" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="O103" s="11" t="s">
         <v>799</v>
@@ -35807,7 +35804,7 @@
         <v>374</v>
       </c>
       <c r="S103" s="11" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="T103" s="11" t="s">
         <v>1265</v>
@@ -35844,7 +35841,7 @@
         <v>1209</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="K104" s="22" t="s">
         <v>1413</v>
@@ -36040,7 +36037,7 @@
         <v>643</v>
       </c>
       <c r="N107" s="11" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="O107" s="14" t="s">
         <v>894</v>
@@ -36055,7 +36052,7 @@
         <v>1832</v>
       </c>
       <c r="S107" s="11" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="T107" s="11" t="s">
         <v>1268</v>
@@ -36071,7 +36068,7 @@
         <v>947</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D108" s="11" t="s">
         <v>877</v>
@@ -36133,7 +36130,7 @@
         <v>952</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D109" s="11" t="s">
         <v>878</v>
@@ -36195,7 +36192,7 @@
         <v>953</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="D110" s="11" t="s">
         <v>879</v>
@@ -36365,7 +36362,7 @@
         <v>377</v>
       </c>
       <c r="S112" s="11" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="T112" s="11" t="s">
         <v>359</v>
@@ -36464,7 +36461,7 @@
         <v>1215</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="K114" s="22" t="s">
         <v>1420</v>
@@ -36489,7 +36486,7 @@
         <v>1693</v>
       </c>
       <c r="S114" s="11" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="T114" s="11" t="s">
         <v>1271</v>
@@ -36588,7 +36585,7 @@
         <v>1217</v>
       </c>
       <c r="J116" s="11" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="K116" s="22" t="s">
         <v>1422</v>
@@ -36675,7 +36672,7 @@
         <v>1695</v>
       </c>
       <c r="S117" s="11" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="T117" s="11" t="s">
         <v>1296</v>
@@ -36712,7 +36709,7 @@
         <v>1218</v>
       </c>
       <c r="J118" s="11" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="K118" s="22" t="s">
         <v>1424</v>
@@ -36737,7 +36734,7 @@
         <v>1696</v>
       </c>
       <c r="S118" s="11" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="T118" s="11" t="s">
         <v>361</v>
@@ -36774,7 +36771,7 @@
         <v>1219</v>
       </c>
       <c r="J119" s="11" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="K119" s="22" t="s">
         <v>1425</v>
@@ -36799,7 +36796,7 @@
         <v>380</v>
       </c>
       <c r="S119" s="11" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="T119" s="11" t="s">
         <v>1274</v>
@@ -37063,7 +37060,7 @@
         <v>232</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="D124" s="11" t="s">
         <v>1308</v>
@@ -37280,7 +37277,7 @@
         <v>658</v>
       </c>
       <c r="N127" s="11" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="O127" s="14" t="s">
         <v>903</v>
@@ -37295,7 +37292,7 @@
         <v>1833</v>
       </c>
       <c r="S127" s="11" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="T127" s="11" t="s">
         <v>1758</v>
@@ -37332,7 +37329,7 @@
         <v>1225</v>
       </c>
       <c r="J128" s="11" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="K128" s="22" t="s">
         <v>1432</v>
@@ -37590,7 +37587,7 @@
         <v>663</v>
       </c>
       <c r="N132" s="11" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="O132" s="14" t="s">
         <v>905</v>
@@ -37605,7 +37602,7 @@
         <v>1700</v>
       </c>
       <c r="S132" s="11" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="T132" s="11" t="s">
         <v>1298</v>
@@ -37683,7 +37680,7 @@
         <v>702</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="D134" s="11" t="s">
         <v>886</v>
@@ -38203,7 +38200,7 @@
         <v>461</v>
       </c>
       <c r="K142" s="22" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="L142" s="22"/>
       <c r="M142" s="22" t="s">
@@ -38277,7 +38274,7 @@
         <v>Mexico City - Summary</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -38290,7 +38287,7 @@
       <c r="L144" s="22"/>
       <c r="M144" s="22"/>
       <c r="N144" s="11" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="O144" s="11"/>
       <c r="P144" s="11"/>
@@ -38345,7 +38342,7 @@
         <v>Phoenix - Summary</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
@@ -38378,7 +38375,7 @@
         <v>Seattle - Summary</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
@@ -38411,7 +38408,7 @@
         <v>Sao Paulo - Summary</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
@@ -38446,7 +38443,7 @@
         <v>Hong Kong - Summary</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11" t="s">
@@ -38538,7 +38535,7 @@
       </c>
       <c r="R151" s="11"/>
       <c r="S151" s="11" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="T151" s="11"/>
       <c r="U151" s="11"/>
@@ -38588,7 +38585,7 @@
         <v>Graz - Summary</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
@@ -38597,7 +38594,7 @@
       <c r="H153" s="11"/>
       <c r="I153" s="22"/>
       <c r="J153" s="11" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="K153" s="22"/>
       <c r="L153" s="22"/>
@@ -38623,7 +38620,7 @@
         <v>Ghent - Summary</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
@@ -38667,7 +38664,7 @@
       <c r="H155" s="11"/>
       <c r="I155" s="22"/>
       <c r="J155" s="11" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="K155" s="22"/>
       <c r="L155" s="22"/>
@@ -38737,7 +38734,7 @@
       <c r="H157" s="11"/>
       <c r="I157" s="22"/>
       <c r="J157" s="11" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="K157" s="22"/>
       <c r="L157" s="22"/>
@@ -38763,7 +38760,7 @@
         <v>Odense - Summary</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
@@ -38798,7 +38795,7 @@
         <v>Barcelona - Summary</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D159" s="11" t="s">
         <v>1769</v>
@@ -38835,7 +38832,7 @@
         <v>Valencia - Summary</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D160" s="11" t="s">
         <v>1770</v>
@@ -38872,7 +38869,7 @@
         <v>Vic - Summary</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D161" s="11" t="s">
         <v>1771</v>
@@ -38909,7 +38906,7 @@
         <v>Belfast - Summary</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
@@ -38975,7 +38972,7 @@
         <v>Adelaide - Summary</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
@@ -39008,7 +39005,7 @@
         <v>Melbourne - Summary</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
@@ -39041,7 +39038,7 @@
         <v>Sydney - Summary</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
@@ -39125,10 +39122,10 @@
         <v>1236</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="N168" s="2" t="s">
         <v>867</v>
@@ -39137,7 +39134,7 @@
         <v>1106</v>
       </c>
       <c r="P168" s="2" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="Q168" s="2" t="s">
         <v>1532</v>
@@ -39381,11 +39378,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAA5C4-0A70-4221-8832-C196189F112B}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39450,10 +39447,10 @@
         <v>1083</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>2009</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39467,7 +39464,7 @@
         <v>1593</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>1646</v>
@@ -39479,10 +39476,10 @@
         <v>1646</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39508,10 +39505,10 @@
         <v>1168</v>
       </c>
       <c r="H4" s="48" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -39537,7 +39534,7 @@
         <v>1169</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>1626</v>
@@ -39566,7 +39563,7 @@
         <v>1827</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>1626</v>
@@ -39595,7 +39592,7 @@
         <v>1590</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>1612</v>
@@ -39609,7 +39606,7 @@
         <v>1785</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1155</v>
@@ -39624,10 +39621,10 @@
         <v>1597</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -39653,10 +39650,10 @@
         <v>1559</v>
       </c>
       <c r="H9" s="48" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39682,10 +39679,10 @@
         <v>1834</v>
       </c>
       <c r="H10" s="48" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39711,10 +39708,10 @@
         <v>1170</v>
       </c>
       <c r="H11" s="48" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39740,10 +39737,10 @@
         <v>1292</v>
       </c>
       <c r="H12" s="48" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -39754,25 +39751,25 @@
         <v>1790</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39798,10 +39795,10 @@
         <v>1645</v>
       </c>
       <c r="H14" s="48" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -39812,25 +39809,25 @@
         <v>1792</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="H15" s="48" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39856,10 +39853,10 @@
         <v>1518</v>
       </c>
       <c r="H16" s="48" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -39870,25 +39867,25 @@
         <v>1794</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -39914,10 +39911,10 @@
         <v>1642</v>
       </c>
       <c r="H18" s="48" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -39943,10 +39940,10 @@
         <v>1159</v>
       </c>
       <c r="H19" s="48" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -39972,10 +39969,10 @@
         <v>1167</v>
       </c>
       <c r="H20" s="48" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -40001,10 +39998,10 @@
         <v>1540</v>
       </c>
       <c r="H21" s="48" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -40030,10 +40027,10 @@
         <v>1162</v>
       </c>
       <c r="H22" s="48" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -40059,10 +40056,10 @@
         <v>1534</v>
       </c>
       <c r="H23" s="48" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="300" x14ac:dyDescent="0.25">
@@ -40073,22 +40070,22 @@
         <v>1799</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="F24" s="20" t="s">
+        <v>1960</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>1961</v>
       </c>
-      <c r="G24" s="20" t="s">
-        <v>1962</v>
-      </c>
       <c r="H24" s="48" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>1626</v>
@@ -40102,7 +40099,7 @@
         <v>1799</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>1164</v>
@@ -40117,7 +40114,7 @@
         <v>1289</v>
       </c>
       <c r="H25" s="48" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>1626</v>
@@ -40131,13 +40128,13 @@
         <v>1799</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="D26" s="20" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E26" s="20" t="s">
         <v>1963</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>1964</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>1538</v>
@@ -40146,7 +40143,7 @@
         <v>1522</v>
       </c>
       <c r="H26" s="48" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>1626</v>
@@ -40175,10 +40172,10 @@
         <v>1536</v>
       </c>
       <c r="H27" s="48" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
     </row>
   </sheetData>
@@ -40627,7 +40624,7 @@
   <dimension ref="A2:U29"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O24" activeCellId="17" sqref="E4:E28 F20:F22 G10:H10 I19 J15 L18 L16 L14 K4 N9 P5 R11 S12 T13 Q20 Q21 Q22 O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40764,7 +40761,7 @@
         <v>818</v>
       </c>
       <c r="K4" s="41" t="s">
-        <v>1837</v>
+        <v>817</v>
       </c>
       <c r="L4" s="37" t="s">
         <v>818</v>
@@ -41240,7 +41237,7 @@
         <v>818</v>
       </c>
       <c r="R11" s="41" t="s">
-        <v>1837</v>
+        <v>817</v>
       </c>
       <c r="S11" s="38" t="s">
         <v>818</v>
@@ -42358,7 +42355,7 @@
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U29" s="2" t="str">
         <f>COUNTIF(E4:T28,"Yes")&amp;"/"&amp;COUNTIF(E4:T28,"&lt;&gt;-")&amp;" reports for "&amp;COUNTA(A4:A28)&amp;" cities across "&amp;COUNTA(E3:T3)&amp;" languages"</f>
-        <v>43/47 reports for 25 cities across 16 languages</v>
+        <v>45/47 reports for 25 cities across 16 languages</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected checkbox iteration in pdf generation
</commit_message>
<xml_diff>
--- a/_report_configuration.xlsx
+++ b/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3590" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F59C73C8-5656-4B52-8044-6E11CB4A6263}"/>
+  <xr:revisionPtr revIDLastSave="3591" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE7FB8E8-2C12-4748-BB2B-13F70055B76E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_web" sheetId="1" r:id="rId1"/>
@@ -7873,11 +7873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V194"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A77" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13375,7 +13375,7 @@
         <v>221</v>
       </c>
       <c r="F93">
-        <f t="shared" si="8"/>
+        <f>F84</f>
         <v>210</v>
       </c>
       <c r="G93">
@@ -30925,11 +30925,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>